<commit_message>
fix delete movimento; relatorio
</commit_message>
<xml_diff>
--- a/Relatorio.xlsx
+++ b/Relatorio.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ainet\projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ainet\proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D46DFA-8627-46B7-87E7-E9989316B3B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7622D6F3-64E4-4F27-99FF-9BA7BE4EE9E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="r4nu9Ssdyn72ILa6XbtalE42PurdRQmxRqHxzo4atH0UewdE3DlkXcEp4UjmR6dvzrejvdX+lgJ5anmpyEOIJQ==" workbookSaltValue="lHIEEz18LbXEtJsTJI7DEA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="129">
   <si>
     <t>Nº Grupo</t>
   </si>
@@ -169,9 +169,6 @@
   </si>
   <si>
     <t>Peso</t>
-  </si>
-  <si>
-    <t>Ignorado</t>
   </si>
   <si>
     <t>Observações Gerais</t>
@@ -522,6 +519,12 @@
   </si>
   <si>
     <t>FAIL: A lista de sócios não tem botões ou hiperlinks para ativar/desativar um sócio -&gt; Existe o botão; FAIL: A lista de sócios não tem nenhum botão ou hiperlink para desativar todos os sócios sem quotas -&gt; Existe o botão</t>
+  </si>
+  <si>
+    <t>Parcial</t>
+  </si>
+  <si>
+    <t>Falta a parte de poder selecionar mais do que um movimento para confirmar</t>
   </si>
 </sst>
 </file>
@@ -801,6 +804,55 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -824,55 +876,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1218,29 +1221,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43:E43"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F51" sqref="F51:I51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="22.15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="22.2" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.75" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.75" style="2" customWidth="1"/>
-    <col min="4" max="4" width="2.25" style="2" customWidth="1"/>
-    <col min="5" max="5" width="6.25" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.75" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.69921875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.69921875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="2.19921875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="6.19921875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.69921875" style="2" customWidth="1"/>
     <col min="7" max="7" width="2.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="6.5" style="2" customWidth="1"/>
     <col min="9" max="9" width="82.5" style="2" customWidth="1"/>
-    <col min="10" max="11" width="7.75" style="2" customWidth="1"/>
-    <col min="12" max="12" width="78.75" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="10.75" style="2"/>
+    <col min="10" max="11" width="7.69921875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="78.69921875" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="10.69921875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1248,19 +1251,19 @@
         <v>27</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="2:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1271,18 +1274,18 @@
         <v>3</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-    </row>
-    <row r="6" spans="2:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+    </row>
+    <row r="6" spans="2:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
@@ -1293,18 +1296,18 @@
         <v>3</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-    </row>
-    <row r="7" spans="2:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+    </row>
+    <row r="7" spans="2:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>1</v>
       </c>
@@ -1315,148 +1318,148 @@
         <v>3</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-    </row>
-    <row r="9" spans="2:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="41" t="s">
+      <c r="I7" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+    </row>
+    <row r="9" spans="2:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-    </row>
-    <row r="10" spans="2:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-    </row>
-    <row r="11" spans="2:11" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-    </row>
-    <row r="12" spans="2:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-    </row>
-    <row r="13" spans="2:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+    </row>
+    <row r="10" spans="2:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+    </row>
+    <row r="11" spans="2:11" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+    </row>
+    <row r="12" spans="2:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+    </row>
+    <row r="13" spans="2:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="14"/>
     </row>
-    <row r="14" spans="2:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="2:11" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
-    </row>
-    <row r="16" spans="2:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
+    </row>
+    <row r="16" spans="2:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="8"/>
       <c r="C16" s="16"/>
     </row>
-    <row r="17" spans="2:12" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="14"/>
+    </row>
+    <row r="18" spans="2:12" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="14"/>
-    </row>
-    <row r="18" spans="2:12" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="2:12" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-    </row>
-    <row r="21" spans="2:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-    </row>
-    <row r="22" spans="2:12" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+    </row>
+    <row r="21" spans="2:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+    </row>
+    <row r="22" spans="2:12" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="27" t="s">
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="17" t="s">
         <v>49</v>
-      </c>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="17" t="s">
-        <v>50</v>
       </c>
       <c r="K22" s="18" t="s">
         <v>44</v>
@@ -1465,1077 +1468,1000 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="D23" s="35"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="39"/>
+      <c r="C23" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" s="24"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="28"/>
       <c r="J23" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K23" s="19">
         <v>1</v>
       </c>
       <c r="L23" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="D24" s="35"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="39"/>
+      <c r="C24" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="24"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="28"/>
       <c r="J24" s="19"/>
       <c r="K24" s="19">
         <v>1</v>
       </c>
       <c r="L24" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="39"/>
+      <c r="C25" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="24"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="28"/>
       <c r="J25" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K25" s="19">
         <v>1</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="D26" s="35"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="39"/>
+      <c r="C26" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="24"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="28"/>
       <c r="J26" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K26" s="19">
         <v>1</v>
       </c>
       <c r="L26" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" s="24"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="D27" s="35"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="39"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="28"/>
       <c r="J27" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K27" s="19">
         <v>1</v>
       </c>
       <c r="L27" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="D28" s="35"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="39"/>
+      <c r="C28" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="24"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="28"/>
       <c r="J28" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K28" s="19">
         <v>2</v>
       </c>
       <c r="L28" s="13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="D29" s="35"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="37" t="s">
-        <v>120</v>
-      </c>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="39"/>
+      <c r="C29" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="24"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="28"/>
       <c r="J29" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K29" s="19">
         <v>3</v>
       </c>
       <c r="L29" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="D30" s="35"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="39"/>
+      <c r="C30" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" s="24"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="28"/>
       <c r="J30" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K30" s="19">
         <v>2</v>
       </c>
       <c r="L30" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
+      <c r="C31" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
       <c r="J31" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K31" s="19">
         <v>3</v>
       </c>
       <c r="L31" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
+      <c r="C32" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
       <c r="J32" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K32" s="19">
         <v>1</v>
       </c>
       <c r="L32" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
+      <c r="C33" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
       <c r="J33" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K33" s="19">
         <v>3</v>
       </c>
       <c r="L33" s="13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
+      <c r="C34" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
       <c r="J34" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K34" s="19">
         <v>4</v>
       </c>
       <c r="L34" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
+      <c r="C35" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
       <c r="J35" s="19"/>
       <c r="K35" s="19">
         <v>6</v>
       </c>
       <c r="L35" s="13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
+      <c r="C36" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
       <c r="J36" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K36" s="19">
         <v>2</v>
       </c>
       <c r="L36" s="13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="31"/>
+      <c r="C37" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
       <c r="J37" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K37" s="19">
         <v>3</v>
       </c>
       <c r="L37" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="32" t="s">
+      <c r="C38" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="31"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="33"/>
       <c r="J38" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K38" s="19">
         <v>4</v>
       </c>
       <c r="L38" s="13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="32" t="s">
+      <c r="C39" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="31"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="33"/>
       <c r="J39" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K39" s="19">
         <v>2</v>
       </c>
       <c r="L39" s="13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="32" t="s">
+      <c r="C40" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="31"/>
-      <c r="I40" s="31"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
       <c r="J40" s="19"/>
       <c r="K40" s="19">
         <v>3</v>
       </c>
       <c r="L40" s="13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C41" s="32" t="s">
+      <c r="C41" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="31"/>
-      <c r="I41" s="31"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="33"/>
       <c r="J41" s="19"/>
       <c r="K41" s="19">
         <v>4</v>
       </c>
       <c r="L41" s="13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C42" s="32" t="s">
+      <c r="C42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="31"/>
-      <c r="I42" s="31"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="33"/>
+      <c r="I42" s="33"/>
       <c r="J42" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K42" s="19">
         <v>1</v>
       </c>
       <c r="L42" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="D43" s="32"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="31"/>
-      <c r="I43" s="31"/>
+      <c r="C43" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
       <c r="J43" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K43" s="19">
         <v>3</v>
       </c>
       <c r="L43" s="13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="32" t="s">
+      <c r="C44" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="31"/>
-      <c r="I44" s="31"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="33"/>
       <c r="J44" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K44" s="19">
         <v>3</v>
       </c>
       <c r="L44" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C45" s="32" t="s">
+      <c r="C45" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="31"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="33"/>
       <c r="J45" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K45" s="19">
         <v>1</v>
       </c>
       <c r="L45" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="32" t="s">
+      <c r="C46" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="31"/>
-      <c r="I46" s="31"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="33"/>
+      <c r="I46" s="33"/>
       <c r="J46" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K46" s="19">
         <v>3</v>
       </c>
       <c r="L46" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C47" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="31"/>
-      <c r="H47" s="31"/>
-      <c r="I47" s="31"/>
+      <c r="C47" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" s="34"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="33"/>
+      <c r="I47" s="33"/>
       <c r="J47" s="19"/>
       <c r="K47" s="19">
         <v>1</v>
       </c>
       <c r="L47" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="48" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C48" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="G48" s="31"/>
-      <c r="H48" s="31"/>
-      <c r="I48" s="31"/>
+      <c r="C48" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="G48" s="33"/>
+      <c r="H48" s="33"/>
+      <c r="I48" s="33"/>
       <c r="J48" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K48" s="19">
         <v>2</v>
       </c>
       <c r="L48" s="13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="49" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C49" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="G49" s="31"/>
-      <c r="H49" s="31"/>
-      <c r="I49" s="31"/>
+      <c r="C49" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D49" s="34"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="G49" s="33"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="33"/>
       <c r="J49" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K49" s="19">
         <v>2</v>
       </c>
       <c r="L49" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="50" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C50" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="31"/>
-      <c r="H50" s="31"/>
-      <c r="I50" s="31"/>
+      <c r="C50" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" s="34"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="33"/>
+      <c r="I50" s="33"/>
       <c r="J50" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K50" s="19">
         <v>2</v>
       </c>
       <c r="L50" s="13" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="51" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C51" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="31"/>
-      <c r="G51" s="31"/>
-      <c r="H51" s="31"/>
-      <c r="I51" s="31"/>
+      <c r="C51" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="D51" s="34"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="G51" s="33"/>
+      <c r="H51" s="33"/>
+      <c r="I51" s="33"/>
       <c r="J51" s="19"/>
       <c r="K51" s="19">
         <v>4</v>
       </c>
       <c r="L51" s="13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="52" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="31"/>
-      <c r="H52" s="31"/>
-      <c r="I52" s="31"/>
+      <c r="C52" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D52" s="34"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="33"/>
+      <c r="H52" s="33"/>
+      <c r="I52" s="33"/>
       <c r="J52" s="19"/>
       <c r="K52" s="19">
         <v>3</v>
       </c>
       <c r="L52" s="13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="53" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C53" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="D53" s="32"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="31"/>
-      <c r="G53" s="31"/>
-      <c r="H53" s="31"/>
-      <c r="I53" s="31"/>
+      <c r="C53" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="33"/>
+      <c r="G53" s="33"/>
+      <c r="H53" s="33"/>
+      <c r="I53" s="33"/>
       <c r="J53" s="19"/>
       <c r="K53" s="19">
         <v>1</v>
       </c>
       <c r="L53" s="13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="54" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C54" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="D54" s="32"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="31"/>
-      <c r="H54" s="31"/>
-      <c r="I54" s="31"/>
+      <c r="C54" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D54" s="34"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="33"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="33"/>
+      <c r="I54" s="33"/>
       <c r="J54" s="19"/>
       <c r="K54" s="19">
         <v>4</v>
       </c>
       <c r="L54" s="13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="55" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C55" s="32" t="s">
+      <c r="C55" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="31"/>
-      <c r="G55" s="31"/>
-      <c r="H55" s="31"/>
-      <c r="I55" s="31"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="33"/>
+      <c r="G55" s="33"/>
+      <c r="H55" s="33"/>
+      <c r="I55" s="33"/>
       <c r="J55" s="19"/>
       <c r="K55" s="19">
         <v>8</v>
       </c>
       <c r="L55" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="57" spans="2:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="C57" s="37"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="37"/>
+      <c r="J57" s="37"/>
+      <c r="K57" s="37"/>
+    </row>
+    <row r="58" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="24"/>
-      <c r="H57" s="24"/>
-      <c r="I57" s="24"/>
-      <c r="J57" s="24"/>
-      <c r="K57" s="24"/>
-    </row>
-    <row r="58" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+      <c r="C58" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D58" s="34"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="33"/>
+      <c r="H58" s="33"/>
+      <c r="I58" s="33"/>
+      <c r="J58" s="41"/>
+      <c r="K58" s="41">
+        <v>15</v>
+      </c>
+      <c r="L58" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C58" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="D58" s="32"/>
-      <c r="E58" s="32"/>
-      <c r="F58" s="31"/>
-      <c r="G58" s="31"/>
-      <c r="H58" s="31"/>
-      <c r="I58" s="31"/>
-      <c r="J58" s="28"/>
-      <c r="K58" s="28">
-        <v>15</v>
-      </c>
-      <c r="L58" s="13" t="s">
+      <c r="C59" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D59" s="34"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="33"/>
+      <c r="G59" s="33"/>
+      <c r="H59" s="33"/>
+      <c r="I59" s="33"/>
+      <c r="J59" s="42"/>
+      <c r="K59" s="42"/>
+      <c r="L59" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
+    <row r="60" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C59" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="D59" s="32"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="31"/>
-      <c r="G59" s="31"/>
-      <c r="H59" s="31"/>
-      <c r="I59" s="31"/>
-      <c r="J59" s="29"/>
-      <c r="K59" s="29"/>
-      <c r="L59" s="13" t="s">
+      <c r="C60" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D60" s="34"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="33"/>
+      <c r="G60" s="33"/>
+      <c r="H60" s="33"/>
+      <c r="I60" s="33"/>
+      <c r="J60" s="42"/>
+      <c r="K60" s="42"/>
+      <c r="L60" s="13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
+    <row r="61" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C60" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="D60" s="32"/>
-      <c r="E60" s="32"/>
-      <c r="F60" s="31"/>
-      <c r="G60" s="31"/>
-      <c r="H60" s="31"/>
-      <c r="I60" s="31"/>
-      <c r="J60" s="29"/>
-      <c r="K60" s="29"/>
-      <c r="L60" s="13" t="s">
+      <c r="C61" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="33"/>
+      <c r="G61" s="33"/>
+      <c r="H61" s="33"/>
+      <c r="I61" s="33"/>
+      <c r="J61" s="42"/>
+      <c r="K61" s="42"/>
+      <c r="L61" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C62" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D62" s="34"/>
+      <c r="E62" s="34"/>
+      <c r="F62" s="33"/>
+      <c r="G62" s="33"/>
+      <c r="H62" s="33"/>
+      <c r="I62" s="33"/>
+      <c r="J62" s="42"/>
+      <c r="K62" s="42"/>
+      <c r="L62" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="61" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C61" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="D61" s="32"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="31"/>
-      <c r="G61" s="31"/>
-      <c r="H61" s="31"/>
-      <c r="I61" s="31"/>
-      <c r="J61" s="29"/>
-      <c r="K61" s="29"/>
-      <c r="L61" s="13" t="s">
+    <row r="63" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C63" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D63" s="34"/>
+      <c r="E63" s="34"/>
+      <c r="F63" s="33"/>
+      <c r="G63" s="33"/>
+      <c r="H63" s="33"/>
+      <c r="I63" s="33"/>
+      <c r="J63" s="42"/>
+      <c r="K63" s="42"/>
+      <c r="L63" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C62" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="31"/>
-      <c r="G62" s="31"/>
-      <c r="H62" s="31"/>
-      <c r="I62" s="31"/>
-      <c r="J62" s="29"/>
-      <c r="K62" s="29"/>
-      <c r="L62" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="63" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
+    <row r="64" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C63" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="D63" s="32"/>
-      <c r="E63" s="32"/>
-      <c r="F63" s="31"/>
-      <c r="G63" s="31"/>
-      <c r="H63" s="31"/>
-      <c r="I63" s="31"/>
-      <c r="J63" s="29"/>
-      <c r="K63" s="29"/>
-      <c r="L63" s="13" t="s">
+      <c r="C64" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D64" s="34"/>
+      <c r="E64" s="34"/>
+      <c r="F64" s="33"/>
+      <c r="G64" s="33"/>
+      <c r="H64" s="33"/>
+      <c r="I64" s="33"/>
+      <c r="J64" s="42"/>
+      <c r="K64" s="42"/>
+      <c r="L64" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
+    <row r="65" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C64" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="D64" s="32"/>
-      <c r="E64" s="32"/>
-      <c r="F64" s="31"/>
-      <c r="G64" s="31"/>
-      <c r="H64" s="31"/>
-      <c r="I64" s="31"/>
-      <c r="J64" s="29"/>
-      <c r="K64" s="29"/>
-      <c r="L64" s="13" t="s">
+      <c r="C65" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D65" s="34"/>
+      <c r="E65" s="34"/>
+      <c r="F65" s="33"/>
+      <c r="G65" s="33"/>
+      <c r="H65" s="33"/>
+      <c r="I65" s="33"/>
+      <c r="J65" s="42"/>
+      <c r="K65" s="42"/>
+      <c r="L65" s="13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
+    <row r="66" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C65" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="D65" s="32"/>
-      <c r="E65" s="32"/>
-      <c r="F65" s="31"/>
-      <c r="G65" s="31"/>
-      <c r="H65" s="31"/>
-      <c r="I65" s="31"/>
-      <c r="J65" s="29"/>
-      <c r="K65" s="29"/>
-      <c r="L65" s="13" t="s">
+      <c r="C66" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D66" s="34"/>
+      <c r="E66" s="34"/>
+      <c r="F66" s="33"/>
+      <c r="G66" s="33"/>
+      <c r="H66" s="33"/>
+      <c r="I66" s="33"/>
+      <c r="J66" s="42"/>
+      <c r="K66" s="42"/>
+      <c r="L66" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="66" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
+    <row r="67" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C66" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="D66" s="32"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="31"/>
-      <c r="G66" s="31"/>
-      <c r="H66" s="31"/>
-      <c r="I66" s="31"/>
-      <c r="J66" s="29"/>
-      <c r="K66" s="29"/>
-      <c r="L66" s="13" t="s">
+      <c r="C67" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D67" s="34"/>
+      <c r="E67" s="34"/>
+      <c r="F67" s="33"/>
+      <c r="G67" s="33"/>
+      <c r="H67" s="33"/>
+      <c r="I67" s="33"/>
+      <c r="J67" s="42"/>
+      <c r="K67" s="42"/>
+      <c r="L67" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
+    <row r="68" spans="2:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C67" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="D67" s="32"/>
-      <c r="E67" s="32"/>
-      <c r="F67" s="31"/>
-      <c r="G67" s="31"/>
-      <c r="H67" s="31"/>
-      <c r="I67" s="31"/>
-      <c r="J67" s="29"/>
-      <c r="K67" s="29"/>
-      <c r="L67" s="13" t="s">
+      <c r="C68" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D68" s="34"/>
+      <c r="E68" s="34"/>
+      <c r="F68" s="33"/>
+      <c r="G68" s="33"/>
+      <c r="H68" s="33"/>
+      <c r="I68" s="33"/>
+      <c r="J68" s="43"/>
+      <c r="K68" s="43"/>
+      <c r="L68" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="68" spans="2:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
+    <row r="70" spans="2:12" s="21" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="22" t="s">
         <v>109</v>
-      </c>
-      <c r="C68" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="D68" s="32"/>
-      <c r="E68" s="32"/>
-      <c r="F68" s="31"/>
-      <c r="G68" s="31"/>
-      <c r="H68" s="31"/>
-      <c r="I68" s="31"/>
-      <c r="J68" s="30"/>
-      <c r="K68" s="30"/>
-      <c r="L68" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="70" spans="2:12" s="21" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="22" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="IN93kqyljkoEgClofw0Q7Or+OqrukMkref6wORKIReYkyivvK6rg1GR3bdW7P+uG208P8Qs0LzJfOpcLuDt2qQ==" saltValue="hnqcxFO1TtfD2N63/RW6dw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="103">
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="B9:I9"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B12:I12"/>
-    <mergeCell ref="B15:K15"/>
-    <mergeCell ref="B11:K11"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="F55:I55"/>
     <mergeCell ref="I5:K5"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="I7:K7"/>
@@ -2560,6 +2486,85 @@
     <mergeCell ref="F65:I65"/>
     <mergeCell ref="C60:E60"/>
     <mergeCell ref="F60:I60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="B15:K15"/>
+    <mergeCell ref="B11:K11"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="C58:E68">

</xml_diff>